<commit_message>
LV Hardware & BOM Updates
</commit_message>
<xml_diff>
--- a/system_development/Mithril/v0.2/Bill of Materials..xlsx
+++ b/system_development/Mithril/v0.2/Bill of Materials..xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayhe\OneDrive\Documents\GitHub\In-situ-monitoring-of-powder-bed-fusion-additive-manufacturing\system_development\Mithril\v0.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\In-situ-monitoring-of-powder-bed-fusion-additive-manufacturing\system_development\Mithril\v0.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3AA924-1233-48B5-BC61-57AA7D981F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB4AF3-03AC-4842-A05A-FD24502B2BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Cylinder Segment Holder</t>
   </si>
   <si>
-    <t>Head Thing (metal)</t>
-  </si>
-  <si>
     <t>M5 x 20</t>
   </si>
   <si>
@@ -193,6 +190,15 @@
   </si>
   <si>
     <t>Source 1</t>
+  </si>
+  <si>
+    <t>Head Plate (metal)</t>
+  </si>
+  <si>
+    <t>Rubber Seal</t>
+  </si>
+  <si>
+    <t>https://www.grainger.com/product/Buna-N-Round-Cord-Buna-N-6RTT7</t>
   </si>
 </sst>
 </file>
@@ -536,21 +542,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,16 +564,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -578,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -589,7 +595,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -600,7 +606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -611,7 +617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -622,7 +628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -633,7 +639,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -644,7 +650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -655,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -666,18 +672,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,22 +691,22 @@
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -711,7 +717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -722,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -733,9 +739,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -744,158 +750,169 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1">
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
         <v>14</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
         <v>3</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
         <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="B30" s="1">
         <v>2</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -921,8 +938,9 @@
     <hyperlink ref="C27" r:id="rId18" xr:uid="{3C1F6BAB-E456-4AE7-8FA5-FD86B5DA18B9}"/>
     <hyperlink ref="C28" r:id="rId19" xr:uid="{E36A8B82-45C1-4D1D-8ACE-1610F6F40364}"/>
     <hyperlink ref="C29" r:id="rId20" xr:uid="{10F24074-5B35-4864-96D9-0BA807DCAE60}"/>
+    <hyperlink ref="C31" r:id="rId21" xr:uid="{B948F647-1980-4846-BB42-49767B59E7B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>